<commit_message>
add sex.childage to sumstat
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Overall labour market rates.xlsx
+++ b/OUTPUT/DATA/Overall labour market rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Work\Childcare and parental employment\childcare\OUTPUT\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greaterlondonauthority.sharepoint.com/sites/S_IU_GLAEconomics/Shared Documents/General/Micro/Labour Market/Ad hoc work/12. Childcare and employment/R/OUTPUT/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E23A8AC-D8FC-4F5B-8BB6-B9B77CFB6521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3E23A8AC-D8FC-4F5B-8BB6-B9B77CFB6521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D7B2562-8D68-4716-8403-942F03C23F1C}"/>
   <bookViews>
-    <workbookView xWindow="-3735" yWindow="8002" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employment rates" sheetId="4" r:id="rId1"/>
@@ -2647,7 +2647,7 @@
   <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:W17"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="2" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -2861,7 +2861,7 @@
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="str">
         <f t="shared" ref="A14:A43" si="2">$O$9</f>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>3</v>
@@ -2877,76 +2877,76 @@
       </c>
       <c r="F14" s="19" t="str">
         <f t="array" aca="1" ref="F14" ca="1">INDEX(INDIRECT($A14),$E14)</f>
-        <v>0 children</v>
+        <v>2 yrs or less</v>
       </c>
       <c r="G14" s="19" t="str">
         <f ca="1">$A14&amp;"_"&amp;$B14&amp;"_"&amp;$C14&amp;"_"&amp;$D14&amp;"_"&amp;$F14</f>
-        <v>num_children_lfsh_aj22_0_1_0 children</v>
+        <v>child_age_lfsh_aj22_0_1_2 yrs or less</v>
       </c>
       <c r="H14" s="19">
         <f ca="1">MATCH($G14,INDEX(INDIRECT($A$1),0,1),0)</f>
-        <v>315</v>
+        <v>175</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J14" s="19" t="str">
         <f ca="1">$A14&amp;"_"&amp;$B14&amp;"_"&amp;$C14&amp;"_"&amp;$I14&amp;"_"&amp;$F14</f>
-        <v>num_children_lfsh_aj22_0_NA_0 children</v>
+        <v>child_age_lfsh_aj22_0_NA_2 yrs or less</v>
       </c>
       <c r="K14" s="19">
         <f ca="1">MATCH($J14,INDEX(INDIRECT($A$1),0,1),0)</f>
-        <v>478</v>
+        <v>408</v>
       </c>
       <c r="M14" s="12" t="str">
         <f ca="1">IFERROR(F14,"")</f>
-        <v>0 children</v>
+        <v>2 yrs or less</v>
       </c>
       <c r="N14" s="4">
         <f t="array" aca="1" ref="N14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H14,N$4),"")</f>
-        <v>0.76871479020348599</v>
+        <v>0.72993547053541996</v>
       </c>
       <c r="O14" s="16">
         <f t="array" aca="1" ref="O14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H14,O$4),"")</f>
-        <v>1.0016529791104499E-2</v>
+        <v>2.8828367806330801E-2</v>
       </c>
       <c r="P14" s="6">
         <f t="array" aca="1" ref="P14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H14,P$4),"")</f>
-        <v>2700</v>
+        <v>386</v>
       </c>
       <c r="Q14" s="6">
         <f t="array" aca="1" ref="Q14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H14,Q$4),"")</f>
-        <v>3638192</v>
+        <v>619252</v>
       </c>
       <c r="R14" s="7">
         <f t="shared" ref="R14:R43" ca="1" si="3">IFERROR(Q14/SUM($Q$14:$Q$43),"")</f>
-        <v>0.5821229212964304</v>
+        <v>9.9082396767036243E-2</v>
       </c>
       <c r="S14" s="4">
         <f t="array" aca="1" ref="S14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K14,S$4),"")</f>
-        <v>0.74867068774218903</v>
+        <v>0.79665538778459699</v>
       </c>
       <c r="T14" s="16">
         <f t="array" aca="1" ref="T14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K14,T$4),"")</f>
-        <v>3.9312107562098301E-3</v>
+        <v>9.3213229867751095E-3</v>
       </c>
       <c r="U14" s="6">
         <f t="array" aca="1" ref="U14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K14,U$4),"")</f>
-        <v>28499</v>
+        <v>3345</v>
       </c>
       <c r="V14" s="6">
         <f t="array" aca="1" ref="V14" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K14,V$4),"")</f>
-        <v>24010160</v>
+        <v>3800022</v>
       </c>
       <c r="W14" s="7">
         <f ca="1">IFERROR(V14/SUM($V$14:$V$43),"")</f>
-        <v>0.5789724770712994</v>
+        <v>9.1632381886061293E-2</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>3</v>
@@ -2963,76 +2963,76 @@
       </c>
       <c r="F15" s="19" t="str">
         <f t="array" aca="1" ref="F15" ca="1">INDEX(INDIRECT($A15),$E15)</f>
-        <v>1 child</v>
+        <v>3-4 yrs</v>
       </c>
       <c r="G15" s="19" t="str">
         <f t="shared" ref="G15:G43" ca="1" si="4">$A15&amp;"_"&amp;$B15&amp;"_"&amp;$C15&amp;"_"&amp;$D15&amp;"_"&amp;$F15</f>
-        <v>num_children_lfsh_aj22_0_1_1 child</v>
+        <v>child_age_lfsh_aj22_0_1_3-4 yrs</v>
       </c>
       <c r="H15" s="19">
         <f ca="1">MATCH($G15,INDEX(INDIRECT($A$1),0,1),0)</f>
-        <v>317</v>
+        <v>177</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="19" t="str">
         <f t="shared" ref="J15:J43" ca="1" si="5">$A15&amp;"_"&amp;$B15&amp;"_"&amp;$C15&amp;"_"&amp;$I15&amp;"_"&amp;$F15</f>
-        <v>num_children_lfsh_aj22_0_NA_1 child</v>
+        <v>child_age_lfsh_aj22_0_NA_3-4 yrs</v>
       </c>
       <c r="K15" s="19">
         <f t="shared" ref="K15:K43" ca="1" si="6">MATCH($J15,INDEX(INDIRECT($A$1),0,1),0)</f>
-        <v>479</v>
+        <v>409</v>
       </c>
       <c r="M15" s="12" t="str">
         <f t="shared" ref="M15:M18" ca="1" si="7">IFERROR(F15,"")</f>
-        <v>1 child</v>
+        <v>3-4 yrs</v>
       </c>
       <c r="N15" s="4">
         <f t="array" aca="1" ref="N15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H15,N$4),"")</f>
-        <v>0.71929827697147397</v>
+        <v>0.72911529751690796</v>
       </c>
       <c r="O15" s="16">
         <f t="array" aca="1" ref="O15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H15,O$4),"")</f>
-        <v>1.7961054360129299E-2</v>
+        <v>3.34202422554278E-2</v>
       </c>
       <c r="P15" s="6">
         <f t="array" aca="1" ref="P15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H15,P$4),"")</f>
-        <v>849</v>
+        <v>221</v>
       </c>
       <c r="Q15" s="6">
         <f t="array" aca="1" ref="Q15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H15,Q$4),"")</f>
-        <v>1118960</v>
+        <v>328099</v>
       </c>
       <c r="R15" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17903735262291098</v>
+        <v>5.2496940335869442E-2</v>
       </c>
       <c r="S15" s="4">
         <f t="array" aca="1" ref="S15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K15,S$4),"")</f>
-        <v>0.76872070388335301</v>
+        <v>0.78581245355206897</v>
       </c>
       <c r="T15" s="16">
         <f t="array" aca="1" ref="T15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K15,T$4),"")</f>
-        <v>5.8391020246933998E-3</v>
+        <v>1.15874337791374E-2</v>
       </c>
       <c r="U15" s="6">
         <f t="array" aca="1" ref="U15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K15,U$4),"")</f>
-        <v>8243</v>
+        <v>2058</v>
       </c>
       <c r="V15" s="6">
         <f t="array" aca="1" ref="V15" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K15,V$4),"")</f>
-        <v>7662065</v>
+        <v>2161022</v>
       </c>
       <c r="W15" s="7">
         <f t="shared" ref="W15:W43" ca="1" si="8">IFERROR(V15/SUM($V$14:$V$43),"")</f>
-        <v>0.18476031615496546</v>
+        <v>5.2110117564629875E-2</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>3</v>
@@ -3049,76 +3049,76 @@
       </c>
       <c r="F16" s="19" t="str">
         <f t="array" aca="1" ref="F16" ca="1">INDEX(INDIRECT($A16),$E16)</f>
-        <v>2 children</v>
+        <v>4-18 yrs</v>
       </c>
       <c r="G16" s="19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>num_children_lfsh_aj22_0_1_2 children</v>
+        <v>child_age_lfsh_aj22_0_1_4-18 yrs</v>
       </c>
       <c r="H16" s="19">
         <f ca="1">MATCH($G16,INDEX(INDIRECT($A$1),0,1),0)</f>
-        <v>319</v>
+        <v>179</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J16" s="19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>num_children_lfsh_aj22_0_NA_2 children</v>
+        <v>child_age_lfsh_aj22_0_NA_4-18 yrs</v>
       </c>
       <c r="K16" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>480</v>
+        <v>410</v>
       </c>
       <c r="M16" s="12" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2 children</v>
+        <v>4-18 yrs</v>
       </c>
       <c r="N16" s="4">
         <f t="array" aca="1" ref="N16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H16,N$4),"")</f>
-        <v>0.74697518325532097</v>
+        <v>0.69179836161905806</v>
       </c>
       <c r="O16" s="16">
         <f t="array" aca="1" ref="O16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H16,O$4),"")</f>
-        <v>1.6794469343059299E-2</v>
+        <v>1.4232456972953E-2</v>
       </c>
       <c r="P16" s="6">
         <f t="array" aca="1" ref="P16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H16,P$4),"")</f>
-        <v>845</v>
+        <v>1370</v>
       </c>
       <c r="Q16" s="6">
         <f t="array" aca="1" ref="Q16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H16,Q$4),"")</f>
-        <v>1041716</v>
+        <v>1664326</v>
       </c>
       <c r="R16" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16667805357200288</v>
+        <v>0.26629774160066394</v>
       </c>
       <c r="S16" s="4">
         <f t="array" aca="1" ref="S16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K16,S$4),"")</f>
-        <v>0.79310849275151696</v>
+        <v>0.739822239877723</v>
       </c>
       <c r="T16" s="16">
         <f t="array" aca="1" ref="T16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K16,T$4),"")</f>
-        <v>5.5874258095487701E-3</v>
+        <v>4.76112903024017E-3</v>
       </c>
       <c r="U16" s="6">
         <f t="array" aca="1" ref="U16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K16,U$4),"")</f>
-        <v>7893</v>
+        <v>13429</v>
       </c>
       <c r="V16" s="6">
         <f t="array" aca="1" ref="V16" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K16,V$4),"")</f>
-        <v>7074998</v>
+        <v>11499092</v>
       </c>
       <c r="W16" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>0.17060399086613706</v>
+        <v>0.27728502347800943</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>3</v>
@@ -3135,76 +3135,76 @@
       </c>
       <c r="F17" s="19" t="str">
         <f t="array" aca="1" ref="F17" ca="1">INDEX(INDIRECT($A17),$E17)</f>
-        <v>3+ children</v>
+        <v>No children</v>
       </c>
       <c r="G17" s="19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>num_children_lfsh_aj22_0_1_3+ children</v>
+        <v>child_age_lfsh_aj22_0_1_No children</v>
       </c>
       <c r="H17" s="19">
         <f ca="1">MATCH($G17,INDEX(INDIRECT($A$1),0,1),0)</f>
-        <v>321</v>
+        <v>181</v>
       </c>
       <c r="I17" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J17" s="19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>num_children_lfsh_aj22_0_NA_3+ children</v>
+        <v>child_age_lfsh_aj22_0_NA_No children</v>
       </c>
       <c r="K17" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>481</v>
+        <v>411</v>
       </c>
       <c r="M17" s="12" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>3+ children</v>
+        <v>No children</v>
       </c>
       <c r="N17" s="4">
         <f t="array" aca="1" ref="N17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H17,N$4),"")</f>
-        <v>0.57563508728362001</v>
+        <v>0.76871479020348599</v>
       </c>
       <c r="O17" s="16">
         <f t="array" aca="1" ref="O17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H17,O$4),"")</f>
-        <v>3.2122234821010502E-2</v>
+        <v>1.0016529791104499E-2</v>
       </c>
       <c r="P17" s="6">
         <f t="array" aca="1" ref="P17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H17,P$4),"")</f>
-        <v>283</v>
+        <v>2700</v>
       </c>
       <c r="Q17" s="6">
         <f t="array" aca="1" ref="Q17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$H17,Q$4),"")</f>
-        <v>451001</v>
+        <v>3638192</v>
       </c>
       <c r="R17" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>7.216167250865578E-2</v>
+        <v>0.5821229212964304</v>
       </c>
       <c r="S17" s="4">
         <f t="array" aca="1" ref="S17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K17,S$4),"")</f>
-        <v>0.63587020986951104</v>
+        <v>0.74867068774218903</v>
       </c>
       <c r="T17" s="16">
         <f t="array" aca="1" ref="T17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K17,T$4),"")</f>
-        <v>1.20630508407989E-2</v>
+        <v>3.9312107562098301E-3</v>
       </c>
       <c r="U17" s="6">
         <f t="array" aca="1" ref="U17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K17,U$4),"")</f>
-        <v>2696</v>
+        <v>28499</v>
       </c>
       <c r="V17" s="6">
         <f t="array" aca="1" ref="V17" ca="1">IFERROR(INDEX(INDIRECT($A$1),$K17,V$4),"")</f>
-        <v>2723073</v>
+        <v>24010160</v>
       </c>
       <c r="W17" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>6.5663215907598049E-2</v>
+        <v>0.5789724770712994</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>3</v>
@@ -3290,7 +3290,7 @@
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>3</v>
@@ -3376,7 +3376,7 @@
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>3</v>
@@ -3462,7 +3462,7 @@
     <row r="21" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>3</v>
@@ -3548,7 +3548,7 @@
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>3</v>
@@ -3634,7 +3634,7 @@
     <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>3</v>
@@ -3720,7 +3720,7 @@
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>3</v>
@@ -3806,7 +3806,7 @@
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>3</v>
@@ -3892,7 +3892,7 @@
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>3</v>
@@ -3978,7 +3978,7 @@
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>3</v>
@@ -4064,7 +4064,7 @@
     <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>3</v>
@@ -4150,7 +4150,7 @@
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>3</v>
@@ -4236,7 +4236,7 @@
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>3</v>
@@ -4322,7 +4322,7 @@
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>3</v>
@@ -4408,7 +4408,7 @@
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>3</v>
@@ -4494,7 +4494,7 @@
     <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>3</v>
@@ -4580,7 +4580,7 @@
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>3</v>
@@ -4666,7 +4666,7 @@
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>3</v>
@@ -4752,7 +4752,7 @@
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>3</v>
@@ -4838,7 +4838,7 @@
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>3</v>
@@ -4924,7 +4924,7 @@
     <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>3</v>
@@ -5010,7 +5010,7 @@
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>3</v>
@@ -5096,7 +5096,7 @@
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>3</v>
@@ -5182,7 +5182,7 @@
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>3</v>
@@ -5268,7 +5268,7 @@
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>3</v>
@@ -5354,7 +5354,7 @@
     <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>num_children</v>
+        <v>child_age</v>
       </c>
       <c r="B43" s="19" t="s">
         <v>3</v>
@@ -44378,6 +44378,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100535EDF9DD8DBB143AE8CD71BDB6B0E3B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58db4c0cb4a6c8574584e2b7e3b481f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9" xmlns:ns3="fd7425d0-09b7-49b7-b351-1ad2162dc0d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f205f5aa0458c3a5f4d8c0367cd4bd4" ns2:_="" ns3:_="">
     <xsd:import namespace="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
@@ -44620,19 +44629,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0E01DCF-E5DB-428F-9698-FBE65787A995}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2456C7AE-9C7D-4534-89FF-CE8F7C34D902}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2456C7AE-9C7D-4534-89FF-CE8F7C34D902}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0E01DCF-E5DB-428F-9698-FBE65787A995}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
+    <ds:schemaRef ds:uri="fd7425d0-09b7-49b7-b351-1ad2162dc0d7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>